<commit_message>
datasaurus dozen excel file update week 1
</commit_message>
<xml_diff>
--- a/Week 1/Datasaurus Dozen.xlsx
+++ b/Week 1/Datasaurus Dozen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatho\Documents\CCS\DRG610A-W21\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389DCF3B-E893-4D2E-97ED-3BF503B3FCCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A5D3CA-1D1C-45D3-9511-4538D2D721BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EAAEC8C-05D9-43DA-BE45-40F59A7DF945}"/>
   </bookViews>
@@ -77,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,16 +85,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -411,303 +427,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E204EFC1-162E-4E86-85DB-EF0CA0566107}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C3" s="3">
         <v>54.266099784204897</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D3" s="3">
         <v>47.834720624884099</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E3" s="3">
         <v>16.7698249541574</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F3" s="3">
         <v>26.939743418883399</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G3" s="3">
         <v>-6.41283521547448E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C4" s="3">
         <v>54.268730022378897</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D4" s="3">
         <v>47.8308231552178</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E4" s="3">
         <v>16.769239493426699</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F4" s="3">
         <v>26.9357266898859</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G4" s="3">
         <v>-6.8586394257948394E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C5" s="3">
         <v>54.2673197061739</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="3">
         <v>47.837717267218302</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E5" s="3">
         <v>16.760012659672199</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F5" s="3">
         <v>26.930036087830299</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G5" s="3">
         <v>-6.8343356450120296E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C6" s="3">
         <v>54.2632732394366</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="3">
         <v>47.832252816901402</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="3">
         <v>16.7651420391168</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F6" s="3">
         <v>26.935403486939101</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G6" s="3">
         <v>-6.4471852700951696E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C7" s="3">
         <v>54.260303451217602</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="3">
         <v>47.839829208755603</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="3">
         <v>16.767735488432599</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="3">
         <v>26.9301915180855</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G7" s="3">
         <v>-6.0341441993538601E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C8" s="3">
         <v>54.261441783514101</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="3">
         <v>47.830251913635202</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="3">
         <v>16.765897904068499</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="3">
         <v>26.9398762200398</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="3">
         <v>-6.1714837956677801E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C9" s="3">
         <v>54.2688052797415</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="3">
         <v>47.835450203936603</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="3">
         <v>16.7667040161692</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="3">
         <v>26.939997961212899</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="3">
         <v>-6.8504220505866895E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C10" s="3">
         <v>54.267848823366201</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="3">
         <v>47.835896330588199</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="3">
         <v>16.7667589474046</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="3">
         <v>26.9361049316378</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="3">
         <v>-6.8979735360631705E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C11" s="3">
         <v>54.265881785602097</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="3">
         <v>47.831495652024401</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="3">
         <v>16.768852670628501</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="3">
         <v>26.938608070892201</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="3">
         <v>-6.8609206445022095E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C12" s="3">
         <v>54.267341104495102</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="3">
         <v>47.839545225097901</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="3">
         <v>16.7689592162765</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="3">
         <v>26.930274687648499</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="3">
         <v>-6.2961100226823094E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C13" s="3">
         <v>54.269927231027502</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="3">
         <v>47.836987988168801</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="3">
         <v>16.769958611355801</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="3">
         <v>26.937683806973901</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="3">
         <v>-6.9445569598172094E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C14" s="3">
         <v>54.266916301256998</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="3">
         <v>47.831601988006199</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="3">
         <v>16.769999617967301</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="3">
         <v>26.937901927715199</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="3">
         <v>-6.6575230199981003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C15" s="3">
         <v>54.260150334038002</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="3">
         <v>47.839717279160404</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="3">
         <v>16.769957695819301</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="3">
         <v>26.930001686981001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="3">
         <v>-6.5583337310065506E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>